<commit_message>
Updated Test schematic and PCB Design
</commit_message>
<xml_diff>
--- a/Test Stand/Documents/Components Selection.xlsx
+++ b/Test Stand/Documents/Components Selection.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacoi\Documents\GitHub\electronics\Catena di Misura\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacoi\Documents\GitHub\electronics\Test Stand\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A524AD-FCCA-442B-9529-B5C40D886DDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B771CAF7-1E1C-4FD0-91AB-9D9BD47D12B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8FD2BC0E-1192-479B-A82E-14357A549AC7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="284">
   <si>
     <t>Components Selection</t>
   </si>
@@ -679,12 +679,6 @@
   </si>
   <si>
     <t>Termocoppia incollabile</t>
-  </si>
-  <si>
-    <t>-250 a 300</t>
-  </si>
-  <si>
-    <t>Classe 1</t>
   </si>
   <si>
     <t>https://www.tcdirect.it/Default.aspx?level=2&amp;department_id=180/24</t>
@@ -982,6 +976,21 @@
   </si>
   <si>
     <t>https://www.ifm.com/it/it/product/EVS024</t>
+  </si>
+  <si>
+    <t>Termocoppia classe 1 da incollare</t>
+  </si>
+  <si>
+    <t>12mm x 20mm</t>
+  </si>
+  <si>
+    <t>-250 a 300°C</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC Direct 402-718	</t>
   </si>
 </sst>
 </file>
@@ -1617,7 +1626,7 @@
   <dimension ref="A1:J98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="J77" sqref="J77"/>
+      <selection activeCell="J78" sqref="J78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1650,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>6</v>
@@ -1941,7 +1950,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B14" s="3">
         <f>SUM(B5:B13)</f>
@@ -1950,7 +1959,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B15" s="26">
         <f>(B5*H5)++(B6*H6)+(B7*H7)+(B8*H8)+(B9*H9)+(B10*H10)+(B11*H11)+(B12*H12)+(B13*H13)</f>
@@ -1965,7 +1974,7 @@
         <v>57</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>60</v>
@@ -2055,7 +2064,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B21" s="3">
         <f>SUM(B19:B20)</f>
@@ -2064,7 +2073,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B22" s="26">
         <f>(B19*H19)+(B20*H20)</f>
@@ -2080,7 +2089,7 @@
         <v>75</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>78</v>
@@ -2234,7 +2243,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B30" s="3">
         <f>SUM(B26:B29)</f>
@@ -2243,7 +2252,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B31" s="26">
         <f>(B26*H26)+(B27*H27)+(B28*H28)+(B29*H29)</f>
@@ -2255,7 +2264,7 @@
         <v>100</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>114</v>
@@ -2273,7 +2282,7 @@
         <v>65</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I34" s="10" t="s">
         <v>41</v>
@@ -2437,7 +2446,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B40" s="3">
         <f>SUM(B35:B39)</f>
@@ -2446,7 +2455,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B41" s="26">
         <f>(B35*H35)+(B36*H36)+(B38*H38)+(B39*H39)</f>
@@ -2458,7 +2467,7 @@
         <v>141</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C44" s="10" t="s">
         <v>142</v>
@@ -2724,7 +2733,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="45" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B53" s="7">
         <v>2</v>
@@ -2749,12 +2758,12 @@
       </c>
       <c r="I53" s="3"/>
       <c r="J53" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B54" s="8">
         <f>SUM(B45:B53)</f>
@@ -2763,7 +2772,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B55" s="26">
         <f>(B45*H45)+(B46*H46)+(B47*H47)+(B48*H48)+(B49*H49)+(B50*H50)+(B51*H51)+(B52*H52)</f>
@@ -2775,7 +2784,7 @@
         <v>78</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
@@ -2784,17 +2793,17 @@
       </c>
       <c r="B59" s="23"/>
       <c r="C59" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D59" s="10" t="s">
         <v>180</v>
       </c>
       <c r="E59" s="10"/>
       <c r="F59" s="10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H59" s="10" t="s">
         <v>179</v>
@@ -2858,7 +2867,7 @@
       </c>
       <c r="C62" s="17"/>
       <c r="D62" s="20" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>183</v>
@@ -2866,18 +2875,16 @@
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="28">
-        <v>80</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>187</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="I62" s="3"/>
       <c r="J62" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B63" s="6">
         <v>0</v>
@@ -2892,23 +2899,23 @@
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
       <c r="H63" s="28">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="I63" s="3"/>
       <c r="J63" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A64" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="B64" s="6">
+      <c r="A64" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B64" s="7">
         <v>0</v>
       </c>
       <c r="C64" s="17"/>
       <c r="D64" s="20" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>183</v>
@@ -2916,130 +2923,138 @@
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="H64" s="28">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="I64" s="3"/>
       <c r="J64" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A65" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B65" s="7">
-        <v>0</v>
-      </c>
-      <c r="C65" s="17"/>
-      <c r="D65" s="20" t="s">
-        <v>195</v>
+      <c r="A65" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B65" s="6">
+        <v>0</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D65" s="24" t="s">
+        <v>207</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
+      <c r="F65" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>209</v>
+      </c>
       <c r="H65" s="28">
-        <v>40</v>
+        <v>8.5</v>
       </c>
       <c r="I65" s="3"/>
       <c r="J65" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="B66" s="6">
+      <c r="A66" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B66" s="7">
         <v>0</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="D66" s="24" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>183</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="H66" s="28">
-        <v>8.5</v>
+        <v>209</v>
+      </c>
+      <c r="H66" s="32">
+        <v>30</v>
       </c>
       <c r="I66" s="3"/>
-      <c r="J66" t="s">
-        <v>212</v>
+      <c r="J66" s="1" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="B67" s="7">
+      <c r="A67" s="45" t="s">
+        <v>283</v>
+      </c>
+      <c r="B67" s="6">
         <v>0</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>220</v>
+        <v>280</v>
       </c>
       <c r="D67" s="24" t="s">
-        <v>221</v>
+        <v>281</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>183</v>
+        <v>282</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H67" s="32">
-        <v>30</v>
-      </c>
-      <c r="I67" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>279</v>
+      </c>
       <c r="J67" s="1" t="s">
-        <v>219</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="44" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B68" s="5">
         <v>5</v>
       </c>
       <c r="C68" s="43" t="s">
+        <v>259</v>
+      </c>
+      <c r="D68" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D68" s="24" t="s">
-        <v>264</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>263</v>
-      </c>
       <c r="F68" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G68" s="3"/>
       <c r="H68" s="32">
         <v>50</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="22" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B69" s="22"/>
       <c r="C69" s="22"/>
@@ -3052,65 +3067,65 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B70" s="5">
         <v>0</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D70" s="24" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H70" s="28">
         <v>10</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J70" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B71" s="7">
+        <v>0</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D71" s="24" t="s">
         <v>213</v>
-      </c>
-      <c r="B71" s="7">
-        <v>0</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="D71" s="24" t="s">
-        <v>215</v>
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G71" s="3"/>
       <c r="H71" s="28">
         <v>90</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J71" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B72" s="3">
         <f>SUM(B60:B71)</f>
@@ -3120,10 +3135,10 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B73" s="26">
-        <f>(B63*H63)+(B64*H64)+(B65*H65)+(B66*H66)+(B67*H67)+(B68*H68)+(B70*H70)+(B71*H71)</f>
+        <f>(B62*H62)+(B63*H63)+(B64*H64)+(B65*H65)+(B66*H66)+(B68*H68)+(B70*H70)+(B71*H71)</f>
         <v>250</v>
       </c>
       <c r="J73" t="s">
@@ -3132,22 +3147,22 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D76" s="10" t="s">
         <v>142</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G76" s="10"/>
       <c r="H76" s="10" t="s">
@@ -3157,13 +3172,13 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="34" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B77" s="34">
         <v>1</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>155</v>
@@ -3177,21 +3192,21 @@
         <v>40</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="34" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B78" s="34">
         <v>1</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>155</v>
@@ -3200,7 +3215,7 @@
         <v>4</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G78" s="3"/>
       <c r="H78" s="28">
@@ -3208,12 +3223,12 @@
       </c>
       <c r="I78" s="3"/>
       <c r="J78" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B79" s="3">
         <f>SUM(B77:B78)</f>
@@ -3222,7 +3237,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B80" s="26">
         <f>(B77*H77)+(B78*H78)</f>
@@ -3231,23 +3246,23 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C83" s="33" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D83" s="33" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E83" s="33"/>
       <c r="F83" s="33" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G83" s="33" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H83" s="33" t="s">
         <v>179</v>
@@ -3258,93 +3273,93 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="35" t="s">
+        <v>228</v>
+      </c>
+      <c r="B84" s="5">
+        <v>0</v>
+      </c>
+      <c r="C84" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="D84" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="B84" s="5">
-        <v>0</v>
-      </c>
-      <c r="C84" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="E84" s="3"/>
       <c r="F84" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="H84" s="28">
         <v>156</v>
       </c>
       <c r="I84" s="3"/>
       <c r="J84" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="36" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B85" s="6">
         <v>0</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E85" s="3"/>
       <c r="F85" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="H85" s="28">
         <v>68</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J85" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B86" s="7">
         <v>1</v>
       </c>
       <c r="C86" s="38" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E86" s="3"/>
       <c r="F86" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H86" s="28">
         <v>114.87</v>
       </c>
       <c r="I86" s="3"/>
       <c r="J86" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B87" s="3">
         <f>SUM(B84:B86)</f>
@@ -3353,7 +3368,7 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B88" s="26">
         <f>(B84*H84)+(B85*H85)+(B86*H86)</f>
@@ -3362,13 +3377,13 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="15" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B91" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D91" s="10" t="s">
         <v>63</v>
@@ -3385,20 +3400,20 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" s="34" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B92" s="34">
         <v>1</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E92" s="3"/>
       <c r="F92" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G92" s="3"/>
       <c r="H92" s="28">
@@ -3406,12 +3421,12 @@
       </c>
       <c r="I92" s="3"/>
       <c r="J92" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" s="25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B93" s="3">
         <f>SUM(B92:B92)</f>
@@ -3420,7 +3435,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B94" s="26">
         <f>(B92*H92)</f>
@@ -3429,7 +3444,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="39" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B97" s="40">
         <f>B14+B21+B30+B40+B54+B72+B87+B79+B93</f>
@@ -3438,7 +3453,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="41" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B98" s="42">
         <f>B15+B22+B31+B41+B55+B73+B88+B80+B94</f>
@@ -3450,7 +3465,7 @@
     <hyperlink ref="J27" r:id="rId1" xr:uid="{A547992E-247C-4226-A546-82F7C2B28F04}"/>
     <hyperlink ref="J28" r:id="rId2" xr:uid="{A42014F1-C1DA-4B21-B48C-1B2F9DB27B1D}"/>
     <hyperlink ref="J52" r:id="rId3" xr:uid="{DFBA6F32-0412-4B50-811B-09BA3C1D9493}"/>
-    <hyperlink ref="J67" r:id="rId4" xr:uid="{406B602F-D266-4902-8EA9-126F2FE635A8}"/>
+    <hyperlink ref="J66" r:id="rId4" xr:uid="{406B602F-D266-4902-8EA9-126F2FE635A8}"/>
     <hyperlink ref="J29" r:id="rId5" xr:uid="{47FBED16-336B-404D-B6ED-8878D2E97D5F}"/>
     <hyperlink ref="J84" r:id="rId6" xr:uid="{C6F3E7B8-6120-4B60-AF55-84E49BEEBBCF}"/>
     <hyperlink ref="J86" r:id="rId7" xr:uid="{A4DC623B-F17A-4403-B85D-11475DE95F83}"/>

</xml_diff>